<commit_message>
Update analysis category words
</commit_message>
<xml_diff>
--- a/code/analysis_of_embeddings/custom_data/word2vec_analysis_category_of_words.xlsx
+++ b/code/analysis_of_embeddings/custom_data/word2vec_analysis_category_of_words.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/triki/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/triki/Documents/repos/inf399-uib/code/analysis_of_embeddings/custom_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D994AA0-FAF4-E242-BF52-28FAECF6249D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351C2D02-6F37-9949-8B40-8FE957BA9FFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{A88987B1-D88D-EF4E-AE81-8B3CAA91553F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{A88987B1-D88D-EF4E-AE81-8B3CAA91553F}"/>
   </bookViews>
   <sheets>
     <sheet name="video_games" sheetId="1" r:id="rId1"/>
+    <sheet name="foods" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="250">
   <si>
     <t>Name</t>
   </si>
@@ -238,6 +239,552 @@
   </si>
   <si>
     <t>Total War: Warhammer</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Artichoke</t>
+  </si>
+  <si>
+    <t>Arugula</t>
+  </si>
+  <si>
+    <t>Asparagus</t>
+  </si>
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Bamboo Shoots</t>
+  </si>
+  <si>
+    <t>Bean Sprouts</t>
+  </si>
+  <si>
+    <t>Beet</t>
+  </si>
+  <si>
+    <t>Belgian Endive</t>
+  </si>
+  <si>
+    <t>Bell Pepper</t>
+  </si>
+  <si>
+    <t>Broccoli</t>
+  </si>
+  <si>
+    <t>Brussels Sprouts</t>
+  </si>
+  <si>
+    <t>Cabbage</t>
+  </si>
+  <si>
+    <t>Calabash</t>
+  </si>
+  <si>
+    <t>Capers</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Cauliflower</t>
+  </si>
+  <si>
+    <t>Celery</t>
+  </si>
+  <si>
+    <t>Celtuce</t>
+  </si>
+  <si>
+    <t>Chayote</t>
+  </si>
+  <si>
+    <t>Cucumber</t>
+  </si>
+  <si>
+    <t>Daikon Radish</t>
+  </si>
+  <si>
+    <t>Edamame</t>
+  </si>
+  <si>
+    <t>Elephant Garlic</t>
+  </si>
+  <si>
+    <t>Endive</t>
+  </si>
+  <si>
+    <t>Fennel</t>
+  </si>
+  <si>
+    <t>Fiddlehead</t>
+  </si>
+  <si>
+    <t>Galangal</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Ginger</t>
+  </si>
+  <si>
+    <t>Grape Leaves</t>
+  </si>
+  <si>
+    <t>Greens</t>
+  </si>
+  <si>
+    <t>Kale</t>
+  </si>
+  <si>
+    <t>Spinach</t>
+  </si>
+  <si>
+    <t>Swiss Chard</t>
+  </si>
+  <si>
+    <t>Hearts of Palm</t>
+  </si>
+  <si>
+    <t>Horseradish</t>
+  </si>
+  <si>
+    <t>Jícama</t>
+  </si>
+  <si>
+    <t>Kohlrabi</t>
+  </si>
+  <si>
+    <t>Leeks</t>
+  </si>
+  <si>
+    <t>Lemongrass</t>
+  </si>
+  <si>
+    <t>Lettuce</t>
+  </si>
+  <si>
+    <t>Lotus Root</t>
+  </si>
+  <si>
+    <t>Lotus Seed</t>
+  </si>
+  <si>
+    <t>Napa Cabbage</t>
+  </si>
+  <si>
+    <t>Nopales</t>
+  </si>
+  <si>
+    <t>Okra</t>
+  </si>
+  <si>
+    <t>Olive</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Parsley</t>
+  </si>
+  <si>
+    <t>Parsley Root</t>
+  </si>
+  <si>
+    <t>Parsnip</t>
+  </si>
+  <si>
+    <t>Peas</t>
+  </si>
+  <si>
+    <t>Plantain</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Pumpkin</t>
+  </si>
+  <si>
+    <t>Purslane</t>
+  </si>
+  <si>
+    <t>Radicchio</t>
+  </si>
+  <si>
+    <t>Radish</t>
+  </si>
+  <si>
+    <t>Rutabaga</t>
+  </si>
+  <si>
+    <t>Shallots</t>
+  </si>
+  <si>
+    <t>Sweet Potato</t>
+  </si>
+  <si>
+    <t>Taro</t>
+  </si>
+  <si>
+    <t>Tomatillo</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Turnip</t>
+  </si>
+  <si>
+    <t>Water Chestnut</t>
+  </si>
+  <si>
+    <t>Water Spinach</t>
+  </si>
+  <si>
+    <t>Watercress</t>
+  </si>
+  <si>
+    <t>Winter Melon</t>
+  </si>
+  <si>
+    <t>Yams</t>
+  </si>
+  <si>
+    <t>Zucchini</t>
+  </si>
+  <si>
+    <t>Beans</t>
+  </si>
+  <si>
+    <t>Bitter Melon</t>
+  </si>
+  <si>
+    <t>Bok Choy</t>
+  </si>
+  <si>
+    <t>Burdock Root</t>
+  </si>
+  <si>
+    <t>Cassava</t>
+  </si>
+  <si>
+    <t>Celery Root</t>
+  </si>
+  <si>
+    <t>Chinese Broccoli</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Aubergine</t>
+  </si>
+  <si>
+    <t>Green Beans</t>
+  </si>
+  <si>
+    <t>Jerusalem Artichoke</t>
+  </si>
+  <si>
+    <t>Mushrooms</t>
+  </si>
+  <si>
+    <t>Peppers</t>
+  </si>
+  <si>
+    <t>Sea Vegetables</t>
+  </si>
+  <si>
+    <t>Squash</t>
+  </si>
+  <si>
+    <t>Vegetable</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Apricot</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Berries</t>
+  </si>
+  <si>
+    <t>Breadfruit</t>
+  </si>
+  <si>
+    <t>Carob</t>
+  </si>
+  <si>
+    <t>Cherry</t>
+  </si>
+  <si>
+    <t>Citron</t>
+  </si>
+  <si>
+    <t>Coconut</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Dragon Fruit</t>
+  </si>
+  <si>
+    <t>Durian</t>
+  </si>
+  <si>
+    <t>Fig</t>
+  </si>
+  <si>
+    <t>Grapes</t>
+  </si>
+  <si>
+    <t>Grapefruit</t>
+  </si>
+  <si>
+    <t>Guava</t>
+  </si>
+  <si>
+    <t>Jackfruit</t>
+  </si>
+  <si>
+    <t>Jujube</t>
+  </si>
+  <si>
+    <t>Kiwifruit</t>
+  </si>
+  <si>
+    <t>Kumquat</t>
+  </si>
+  <si>
+    <t>Lemon</t>
+  </si>
+  <si>
+    <t>Lime</t>
+  </si>
+  <si>
+    <t>Longan</t>
+  </si>
+  <si>
+    <t>Loquat</t>
+  </si>
+  <si>
+    <t>Lucuma</t>
+  </si>
+  <si>
+    <t>Lychee</t>
+  </si>
+  <si>
+    <t>Mamey Sapote</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Mangosteen</t>
+  </si>
+  <si>
+    <t>Melon</t>
+  </si>
+  <si>
+    <t>Nance</t>
+  </si>
+  <si>
+    <t>Nectarine</t>
+  </si>
+  <si>
+    <t>Noni</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Papaya</t>
+  </si>
+  <si>
+    <t>Passion Fruit</t>
+  </si>
+  <si>
+    <t>Peach</t>
+  </si>
+  <si>
+    <t>Pear</t>
+  </si>
+  <si>
+    <t>Persimmon</t>
+  </si>
+  <si>
+    <t>Pineapple</t>
+  </si>
+  <si>
+    <t>Plum</t>
+  </si>
+  <si>
+    <t>Pomegranate</t>
+  </si>
+  <si>
+    <t>Pomelo</t>
+  </si>
+  <si>
+    <t>Prickly Pear</t>
+  </si>
+  <si>
+    <t>Quince</t>
+  </si>
+  <si>
+    <t>Rambutan</t>
+  </si>
+  <si>
+    <t>Rhubarb</t>
+  </si>
+  <si>
+    <t>Starfruit</t>
+  </si>
+  <si>
+    <t>Tamarillo</t>
+  </si>
+  <si>
+    <t>Tamarind</t>
+  </si>
+  <si>
+    <t>Tangerine</t>
+  </si>
+  <si>
+    <t>Tangelo</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Amaranth</t>
+  </si>
+  <si>
+    <t>Barley</t>
+  </si>
+  <si>
+    <t>Buckwheat</t>
+  </si>
+  <si>
+    <t>Millet</t>
+  </si>
+  <si>
+    <t>Oats</t>
+  </si>
+  <si>
+    <t>Quinoa</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Rye</t>
+  </si>
+  <si>
+    <t>Sorghum</t>
+  </si>
+  <si>
+    <t>Spelt</t>
+  </si>
+  <si>
+    <t>Teff</t>
+  </si>
+  <si>
+    <t>Triticale</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>Acorn</t>
+  </si>
+  <si>
+    <t>Almond</t>
+  </si>
+  <si>
+    <t>Brazil Nut</t>
+  </si>
+  <si>
+    <t>Candlenut</t>
+  </si>
+  <si>
+    <t>Cashew</t>
+  </si>
+  <si>
+    <t>Chestnuts</t>
+  </si>
+  <si>
+    <t>Hazelnut</t>
+  </si>
+  <si>
+    <t>Kola Nut</t>
+  </si>
+  <si>
+    <t>Macadamia</t>
+  </si>
+  <si>
+    <t>Peanut</t>
+  </si>
+  <si>
+    <t>Pecan</t>
+  </si>
+  <si>
+    <t>Pili Nut</t>
+  </si>
+  <si>
+    <t>Pine Nut</t>
+  </si>
+  <si>
+    <t>Pistachio</t>
+  </si>
+  <si>
+    <t>Soynuts</t>
+  </si>
+  <si>
+    <t>Walnut</t>
+  </si>
+  <si>
+    <t>Nuts</t>
+  </si>
+  <si>
+    <t>Caraway Seeds</t>
+  </si>
+  <si>
+    <t>Chia Seeds</t>
+  </si>
+  <si>
+    <t>Flax Seeds</t>
+  </si>
+  <si>
+    <t>Hemp Seeds</t>
+  </si>
+  <si>
+    <t>Poppy Seeds</t>
+  </si>
+  <si>
+    <t>Pumpkin Seeds</t>
+  </si>
+  <si>
+    <t>Sesame Seeds</t>
+  </si>
+  <si>
+    <t>Squash Seeds</t>
+  </si>
+  <si>
+    <t>Sunflower Seeds</t>
+  </si>
+  <si>
+    <t>Seeds</t>
   </si>
 </sst>
 </file>
@@ -600,7 +1147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3552888D-C152-7D47-B69E-CB55FEBC4D34}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -1101,4 +1648,1487 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404FE1F0-EE3D-9540-9CEE-5B4AD9622963}">
+  <dimension ref="A1:B183"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>125</v>
+      </c>
+      <c r="B69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>127</v>
+      </c>
+      <c r="B71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>102</v>
+      </c>
+      <c r="B77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>130</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>131</v>
+      </c>
+      <c r="B79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>134</v>
+      </c>
+      <c r="B82" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>139</v>
+      </c>
+      <c r="B87" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>156</v>
+      </c>
+      <c r="B88" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>157</v>
+      </c>
+      <c r="B89" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>158</v>
+      </c>
+      <c r="B91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>159</v>
+      </c>
+      <c r="B92" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>160</v>
+      </c>
+      <c r="B93" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>161</v>
+      </c>
+      <c r="B94" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>162</v>
+      </c>
+      <c r="B95" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>163</v>
+      </c>
+      <c r="B96" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>164</v>
+      </c>
+      <c r="B97" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>165</v>
+      </c>
+      <c r="B98" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>166</v>
+      </c>
+      <c r="B99" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>167</v>
+      </c>
+      <c r="B100" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>168</v>
+      </c>
+      <c r="B101" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>97</v>
+      </c>
+      <c r="B102" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>169</v>
+      </c>
+      <c r="B103" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>170</v>
+      </c>
+      <c r="B104" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>171</v>
+      </c>
+      <c r="B105" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>172</v>
+      </c>
+      <c r="B106" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>173</v>
+      </c>
+      <c r="B107" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>174</v>
+      </c>
+      <c r="B108" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>175</v>
+      </c>
+      <c r="B109" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>176</v>
+      </c>
+      <c r="B110" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>177</v>
+      </c>
+      <c r="B111" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>179</v>
+      </c>
+      <c r="B113" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>180</v>
+      </c>
+      <c r="B114" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>181</v>
+      </c>
+      <c r="B115" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>182</v>
+      </c>
+      <c r="B116" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>183</v>
+      </c>
+      <c r="B117" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>184</v>
+      </c>
+      <c r="B118" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>185</v>
+      </c>
+      <c r="B119" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>186</v>
+      </c>
+      <c r="B120" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>187</v>
+      </c>
+      <c r="B121" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>188</v>
+      </c>
+      <c r="B122" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>189</v>
+      </c>
+      <c r="B123" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>190</v>
+      </c>
+      <c r="B124" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>191</v>
+      </c>
+      <c r="B125" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>192</v>
+      </c>
+      <c r="B126" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>193</v>
+      </c>
+      <c r="B127" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>194</v>
+      </c>
+      <c r="B128" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>195</v>
+      </c>
+      <c r="B129" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>121</v>
+      </c>
+      <c r="B130" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>196</v>
+      </c>
+      <c r="B131" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>197</v>
+      </c>
+      <c r="B132" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>198</v>
+      </c>
+      <c r="B133" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>199</v>
+      </c>
+      <c r="B134" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>200</v>
+      </c>
+      <c r="B135" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>201</v>
+      </c>
+      <c r="B136" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>202</v>
+      </c>
+      <c r="B137" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>203</v>
+      </c>
+      <c r="B138" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>204</v>
+      </c>
+      <c r="B139" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>205</v>
+      </c>
+      <c r="B140" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>206</v>
+      </c>
+      <c r="B141" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>207</v>
+      </c>
+      <c r="B142" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>132</v>
+      </c>
+      <c r="B143" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>209</v>
+      </c>
+      <c r="B144" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>210</v>
+      </c>
+      <c r="B145" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>211</v>
+      </c>
+      <c r="B146" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>212</v>
+      </c>
+      <c r="B148" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>213</v>
+      </c>
+      <c r="B149" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>214</v>
+      </c>
+      <c r="B150" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>215</v>
+      </c>
+      <c r="B151" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>216</v>
+      </c>
+      <c r="B152" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>217</v>
+      </c>
+      <c r="B153" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>218</v>
+      </c>
+      <c r="B154" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>219</v>
+      </c>
+      <c r="B155" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>220</v>
+      </c>
+      <c r="B156" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>221</v>
+      </c>
+      <c r="B157" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>223</v>
+      </c>
+      <c r="B158" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>224</v>
+      </c>
+      <c r="B159" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>225</v>
+      </c>
+      <c r="B160" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>226</v>
+      </c>
+      <c r="B161" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>227</v>
+      </c>
+      <c r="B162" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>228</v>
+      </c>
+      <c r="B163" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>229</v>
+      </c>
+      <c r="B165" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>230</v>
+      </c>
+      <c r="B166" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>231</v>
+      </c>
+      <c r="B167" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>232</v>
+      </c>
+      <c r="B168" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>233</v>
+      </c>
+      <c r="B169" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>234</v>
+      </c>
+      <c r="B170" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>235</v>
+      </c>
+      <c r="B171" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>236</v>
+      </c>
+      <c r="B172" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>237</v>
+      </c>
+      <c r="B173" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>238</v>
+      </c>
+      <c r="B174" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>240</v>
+      </c>
+      <c r="B175" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>241</v>
+      </c>
+      <c r="B176" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>242</v>
+      </c>
+      <c r="B177" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>243</v>
+      </c>
+      <c r="B178" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>244</v>
+      </c>
+      <c r="B179" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>245</v>
+      </c>
+      <c r="B180" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>246</v>
+      </c>
+      <c r="B181" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>247</v>
+      </c>
+      <c r="B182" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>248</v>
+      </c>
+      <c r="B183" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update utils and custom data
</commit_message>
<xml_diff>
--- a/code/analysis_of_embeddings/custom_data/word2vec_analysis_category_of_words.xlsx
+++ b/code/analysis_of_embeddings/custom_data/word2vec_analysis_category_of_words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/triki/Documents/repos/inf399-uib/code/analysis_of_embeddings/custom_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351C2D02-6F37-9949-8B40-8FE957BA9FFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F2483F-13C7-2041-AC53-A70CE1D30515}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{A88987B1-D88D-EF4E-AE81-8B3CAA91553F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="250">
   <si>
     <t>Name</t>
   </si>
@@ -1652,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404FE1F0-EE3D-9540-9CEE-5B4AD9622963}">
-  <dimension ref="A1:B183"/>
+  <dimension ref="A1:B177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>155</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>155</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
@@ -1722,7 +1722,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
         <v>155</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
         <v>155</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
         <v>155</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
         <v>155</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
         <v>155</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
         <v>155</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
         <v>155</v>
@@ -1778,7 +1778,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
         <v>155</v>
@@ -1786,7 +1786,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
         <v>155</v>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
         <v>155</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>155</v>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
         <v>155</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
         <v>155</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>155</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
         <v>155</v>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="B23" t="s">
         <v>155</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>155</v>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>155</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
         <v>155</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
         <v>155</v>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
         <v>155</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
         <v>155</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
         <v>155</v>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
         <v>155</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
         <v>155</v>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
         <v>155</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
         <v>155</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
         <v>155</v>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>155</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
         <v>155</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
         <v>155</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
         <v>155</v>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
         <v>155</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
         <v>155</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
         <v>155</v>
@@ -2002,7 +2002,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
         <v>155</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
         <v>155</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
         <v>155</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
         <v>155</v>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
         <v>155</v>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
         <v>155</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>155</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B50" t="s">
         <v>155</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
         <v>155</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
         <v>155</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" t="s">
         <v>155</v>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
         <v>155</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
         <v>155</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
         <v>155</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
         <v>155</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
         <v>155</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
         <v>155</v>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B60" t="s">
         <v>155</v>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
         <v>155</v>
@@ -2154,7 +2154,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
         <v>155</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B63" t="s">
         <v>155</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B64" t="s">
         <v>155</v>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
         <v>155</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s">
         <v>155</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B67" t="s">
         <v>155</v>
@@ -2202,7 +2202,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
         <v>155</v>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B69" t="s">
         <v>155</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="B70" t="s">
         <v>155</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B71" t="s">
         <v>155</v>
@@ -2234,7 +2234,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
         <v>155</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="B73" t="s">
         <v>155</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="B74" t="s">
         <v>155</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="B75" t="s">
         <v>155</v>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B76" t="s">
         <v>155</v>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="B77" t="s">
         <v>155</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B78" t="s">
         <v>155</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B79" t="s">
         <v>155</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B80" t="s">
         <v>155</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B81" t="s">
         <v>155</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B82" t="s">
         <v>155</v>
@@ -2322,7 +2322,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B83" t="s">
         <v>155</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B84" t="s">
         <v>155</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B85" t="s">
         <v>155</v>
@@ -2346,23 +2346,23 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="B88" t="s">
         <v>208</v>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B89" t="s">
         <v>208</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>72</v>
+        <v>159</v>
       </c>
       <c r="B90" t="s">
         <v>208</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B91" t="s">
         <v>208</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B92" t="s">
         <v>208</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B93" t="s">
         <v>208</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B94" t="s">
         <v>208</v>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B95" t="s">
         <v>208</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B96" t="s">
         <v>208</v>
@@ -2434,7 +2434,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B97" t="s">
         <v>208</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B98" t="s">
         <v>208</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B99" t="s">
         <v>208</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B100" t="s">
         <v>208</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B101" t="s">
         <v>208</v>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>171</v>
       </c>
       <c r="B102" t="s">
         <v>208</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B103" t="s">
         <v>208</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B104" t="s">
         <v>208</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B105" t="s">
         <v>208</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B106" t="s">
         <v>208</v>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B107" t="s">
         <v>208</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B108" t="s">
         <v>208</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B109" t="s">
         <v>208</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B110" t="s">
         <v>208</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B111" t="s">
         <v>208</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B112" t="s">
         <v>208</v>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B113" t="s">
         <v>208</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B114" t="s">
         <v>208</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B115" t="s">
         <v>208</v>
@@ -2586,7 +2586,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B116" t="s">
         <v>208</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B117" t="s">
         <v>208</v>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B118" t="s">
         <v>208</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B119" t="s">
         <v>208</v>
@@ -2618,7 +2618,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B120" t="s">
         <v>208</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B121" t="s">
         <v>208</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B122" t="s">
         <v>208</v>
@@ -2642,7 +2642,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B123" t="s">
         <v>208</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B124" t="s">
         <v>208</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B125" t="s">
         <v>208</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B126" t="s">
         <v>208</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B127" t="s">
         <v>208</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B128" t="s">
         <v>208</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B129" t="s">
         <v>208</v>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>121</v>
+        <v>199</v>
       </c>
       <c r="B130" t="s">
         <v>208</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B131" t="s">
         <v>208</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B132" t="s">
         <v>208</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B133" t="s">
         <v>208</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B134" t="s">
         <v>208</v>
@@ -2738,7 +2738,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B135" t="s">
         <v>208</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B136" t="s">
         <v>208</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B137" t="s">
         <v>208</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B138" t="s">
         <v>208</v>
@@ -2770,47 +2770,47 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B139" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B140" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B141" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>207</v>
+        <v>147</v>
       </c>
       <c r="B142" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>132</v>
+        <v>212</v>
       </c>
       <c r="B143" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B144" t="s">
         <v>222</v>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B145" t="s">
         <v>222</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B146" t="s">
         <v>222</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="B147" t="s">
         <v>222</v>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B148" t="s">
         <v>222</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B149" t="s">
         <v>222</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B150" t="s">
         <v>222</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B151" t="s">
         <v>222</v>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B152" t="s">
         <v>222</v>
@@ -2882,47 +2882,47 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B153" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B154" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B155" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B156" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B157" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B158" t="s">
         <v>239</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B159" t="s">
         <v>239</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B160" t="s">
         <v>239</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B161" t="s">
         <v>239</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B162" t="s">
         <v>239</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B163" t="s">
         <v>239</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>164</v>
+        <v>234</v>
       </c>
       <c r="B164" t="s">
         <v>239</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B165" t="s">
         <v>239</v>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B166" t="s">
         <v>239</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B167" t="s">
         <v>239</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B168" t="s">
         <v>239</v>
@@ -3010,55 +3010,55 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B169" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="B170" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="B171" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B172" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B173" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="B174" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B175" t="s">
         <v>249</v>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B176" t="s">
         <v>249</v>
@@ -3074,57 +3074,9 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B177" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>243</v>
-      </c>
-      <c r="B178" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>244</v>
-      </c>
-      <c r="B179" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>245</v>
-      </c>
-      <c r="B180" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>246</v>
-      </c>
-      <c r="B181" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>247</v>
-      </c>
-      <c r="B182" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>248</v>
-      </c>
-      <c r="B183" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>